<commit_message>
changes in attribute UI and flow UI
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shivang Dudani\Desktop\ONDC-NTS-Specifications\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DD2F32A-A562-44EA-83BD-380B3581C294}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CAE0409-9352-4EB3-8A0B-8750A18ED7DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="1" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="settle_misc" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1175" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1103" uniqueCount="137">
   <si>
     <t>Path</t>
   </si>
@@ -814,10 +814,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E26"/>
+  <dimension ref="A1:E24"/>
   <sheetViews>
-    <sheetView topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1069,7 +1069,7 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="B15" t="b">
         <v>1</v>
@@ -1081,12 +1081,12 @@
         <v>7</v>
       </c>
       <c r="E15" t="s">
-        <v>18</v>
+        <v>37</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="B16" t="b">
         <v>1</v>
@@ -1098,12 +1098,12 @@
         <v>7</v>
       </c>
       <c r="E16" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="B17" t="b">
         <v>1</v>
@@ -1115,12 +1115,12 @@
         <v>7</v>
       </c>
       <c r="E17" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="B18" t="b">
         <v>1</v>
@@ -1132,12 +1132,12 @@
         <v>7</v>
       </c>
       <c r="E18" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="B19" t="b">
         <v>1</v>
@@ -1149,12 +1149,12 @@
         <v>7</v>
       </c>
       <c r="E19" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="B20" t="b">
         <v>1</v>
@@ -1166,12 +1166,12 @@
         <v>7</v>
       </c>
       <c r="E20" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="B21" t="b">
         <v>1</v>
@@ -1182,13 +1182,13 @@
       <c r="D21" t="s">
         <v>7</v>
       </c>
-      <c r="E21" t="s">
-        <v>45</v>
+      <c r="E21">
+        <v>1234567890</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="B22" t="b">
         <v>1</v>
@@ -1200,12 +1200,12 @@
         <v>7</v>
       </c>
       <c r="E22" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="B23" t="b">
         <v>1</v>
@@ -1216,13 +1216,13 @@
       <c r="D23" t="s">
         <v>7</v>
       </c>
-      <c r="E23">
-        <v>1234567890</v>
+      <c r="E23" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="B24" t="b">
         <v>1</v>
@@ -1234,40 +1234,6 @@
         <v>7</v>
       </c>
       <c r="E24" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A25" t="s">
-        <v>52</v>
-      </c>
-      <c r="B25" t="b">
-        <v>1</v>
-      </c>
-      <c r="C25" t="s">
-        <v>6</v>
-      </c>
-      <c r="D25" t="s">
-        <v>7</v>
-      </c>
-      <c r="E25" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A26" t="s">
-        <v>53</v>
-      </c>
-      <c r="B26" t="b">
-        <v>1</v>
-      </c>
-      <c r="C26" t="s">
-        <v>6</v>
-      </c>
-      <c r="D26" t="s">
-        <v>7</v>
-      </c>
-      <c r="E26" t="s">
         <v>43</v>
       </c>
     </row>
@@ -1824,9 +1790,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:E31"/>
+  <dimension ref="A1:E15"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -2074,7 +2042,7 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="B15" t="b">
         <v>1</v>
@@ -2086,279 +2054,7 @@
         <v>7</v>
       </c>
       <c r="E15" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A16" t="s">
-        <v>34</v>
-      </c>
-      <c r="B16" t="b">
-        <v>1</v>
-      </c>
-      <c r="C16" t="s">
-        <v>6</v>
-      </c>
-      <c r="D16" t="s">
-        <v>7</v>
-      </c>
-      <c r="E16" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A17" t="s">
-        <v>36</v>
-      </c>
-      <c r="B17" t="b">
-        <v>1</v>
-      </c>
-      <c r="C17" t="s">
-        <v>6</v>
-      </c>
-      <c r="D17" t="s">
-        <v>7</v>
-      </c>
-      <c r="E17" t="s">
         <v>67</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A18" t="s">
-        <v>38</v>
-      </c>
-      <c r="B18" t="b">
-        <v>1</v>
-      </c>
-      <c r="C18" t="s">
-        <v>6</v>
-      </c>
-      <c r="D18" t="s">
-        <v>7</v>
-      </c>
-      <c r="E18" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A19" t="s">
-        <v>40</v>
-      </c>
-      <c r="B19" t="b">
-        <v>1</v>
-      </c>
-      <c r="C19" t="s">
-        <v>6</v>
-      </c>
-      <c r="D19" t="s">
-        <v>7</v>
-      </c>
-      <c r="E19" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A20" t="s">
-        <v>42</v>
-      </c>
-      <c r="B20" t="b">
-        <v>1</v>
-      </c>
-      <c r="C20" t="s">
-        <v>6</v>
-      </c>
-      <c r="D20" t="s">
-        <v>7</v>
-      </c>
-      <c r="E20" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A21" t="s">
-        <v>44</v>
-      </c>
-      <c r="B21" t="b">
-        <v>1</v>
-      </c>
-      <c r="C21" t="s">
-        <v>6</v>
-      </c>
-      <c r="D21" t="s">
-        <v>7</v>
-      </c>
-      <c r="E21" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A22" t="s">
-        <v>46</v>
-      </c>
-      <c r="B22" t="b">
-        <v>1</v>
-      </c>
-      <c r="C22" t="s">
-        <v>6</v>
-      </c>
-      <c r="D22" t="s">
-        <v>7</v>
-      </c>
-      <c r="E22" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A23" t="s">
-        <v>48</v>
-      </c>
-      <c r="B23" t="b">
-        <v>1</v>
-      </c>
-      <c r="C23" t="s">
-        <v>6</v>
-      </c>
-      <c r="D23" t="s">
-        <v>7</v>
-      </c>
-      <c r="E23" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A24" t="s">
-        <v>50</v>
-      </c>
-      <c r="B24" t="b">
-        <v>1</v>
-      </c>
-      <c r="C24" t="s">
-        <v>6</v>
-      </c>
-      <c r="D24" t="s">
-        <v>7</v>
-      </c>
-      <c r="E24" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A25" t="s">
-        <v>52</v>
-      </c>
-      <c r="B25" t="b">
-        <v>1</v>
-      </c>
-      <c r="C25" t="s">
-        <v>6</v>
-      </c>
-      <c r="D25" t="s">
-        <v>7</v>
-      </c>
-      <c r="E25" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A26" t="s">
-        <v>53</v>
-      </c>
-      <c r="B26" t="b">
-        <v>1</v>
-      </c>
-      <c r="C26" t="s">
-        <v>6</v>
-      </c>
-      <c r="D26" t="s">
-        <v>7</v>
-      </c>
-      <c r="E26" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A27" t="s">
-        <v>59</v>
-      </c>
-      <c r="B27" t="b">
-        <v>1</v>
-      </c>
-      <c r="C27" t="s">
-        <v>6</v>
-      </c>
-      <c r="D27" t="s">
-        <v>7</v>
-      </c>
-      <c r="E27" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A28" t="s">
-        <v>61</v>
-      </c>
-      <c r="B28" t="b">
-        <v>1</v>
-      </c>
-      <c r="C28" t="s">
-        <v>6</v>
-      </c>
-      <c r="D28" t="s">
-        <v>7</v>
-      </c>
-      <c r="E28" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A29" t="s">
-        <v>62</v>
-      </c>
-      <c r="B29" t="b">
-        <v>1</v>
-      </c>
-      <c r="C29" t="s">
-        <v>6</v>
-      </c>
-      <c r="D29" t="s">
-        <v>7</v>
-      </c>
-      <c r="E29" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A30" t="s">
-        <v>64</v>
-      </c>
-      <c r="B30" t="b">
-        <v>1</v>
-      </c>
-      <c r="C30" t="s">
-        <v>6</v>
-      </c>
-      <c r="D30" t="s">
-        <v>7</v>
-      </c>
-      <c r="E30" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A31" t="s">
-        <v>65</v>
-      </c>
-      <c r="B31" t="b">
-        <v>1</v>
-      </c>
-      <c r="C31" t="s">
-        <v>6</v>
-      </c>
-      <c r="D31" t="s">
-        <v>7</v>
-      </c>
-      <c r="E31" t="s">
-        <v>66</v>
       </c>
     </row>
   </sheetData>
@@ -5287,7 +4983,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A61EBF98-981C-4233-B839-BBDDE82D6C34}">
   <dimension ref="A1:E38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+    <sheetView topLeftCell="A22" workbookViewId="0">
       <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
due date added when recon_accord is true
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10916"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11207"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shivangdudani/Desktop/ONDC-NTS-Specifications/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shahi/Developer/ONDC-NTS-Specifications/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0694D88F-3C83-F44C-9544-6D87C05D6C77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95C98283-1600-A042-8B96-7554B475E52B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="19420" windowHeight="10300" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="18380" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="settle_misc" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1378" uniqueCount="212">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1383" uniqueCount="215">
   <si>
     <t>Path</t>
   </si>
@@ -663,6 +663,15 @@
   </si>
   <si>
     <t>Currency of the amount that is to be settled from collector to receiver</t>
+  </si>
+  <si>
+    <t>message.orders.settlements.due_date</t>
+  </si>
+  <si>
+    <t>due date of settlement in case recon_accord is true</t>
+  </si>
+  <si>
+    <t>2024-05-09</t>
   </si>
 </sst>
 </file>
@@ -772,7 +781,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -787,6 +796,7 @@
     <xf numFmtId="49" fontId="3" fillId="2" borderId="3" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="3" fillId="2" borderId="4" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="3" fillId="2" borderId="0" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -5318,7 +5328,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2020830-4AD2-4262-A507-560AC4C1F264}">
   <dimension ref="A1:F32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+    <sheetView topLeftCell="A18" workbookViewId="0">
       <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
@@ -5980,10 +5990,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A61EBF98-981C-4233-B839-BBDDE82D6C34}">
-  <dimension ref="A1:F38"/>
+  <dimension ref="A1:F39"/>
   <sheetViews>
-    <sheetView topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="F38" sqref="F38"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -6535,10 +6545,10 @@
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>111</v>
+        <v>212</v>
       </c>
       <c r="B28" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C28" t="s">
         <v>6</v>
@@ -6546,19 +6556,19 @@
       <c r="D28" t="s">
         <v>7</v>
       </c>
-      <c r="E28" t="s">
-        <v>41</v>
-      </c>
-      <c r="F28" t="s">
-        <v>185</v>
+      <c r="E28" s="8" t="s">
+        <v>214</v>
+      </c>
+      <c r="F28" s="7" t="s">
+        <v>213</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B29" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C29" t="s">
         <v>6</v>
@@ -6566,19 +6576,19 @@
       <c r="D29" t="s">
         <v>7</v>
       </c>
-      <c r="E29" s="2" t="s">
-        <v>132</v>
+      <c r="E29" t="s">
+        <v>41</v>
       </c>
       <c r="F29" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>121</v>
+        <v>112</v>
       </c>
       <c r="B30" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C30" t="s">
         <v>6</v>
@@ -6587,15 +6597,15 @@
         <v>7</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>126</v>
+        <v>132</v>
       </c>
       <c r="F30" t="s">
-        <v>201</v>
+        <v>186</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>113</v>
+        <v>121</v>
       </c>
       <c r="B31" t="b">
         <v>1</v>
@@ -6606,19 +6616,19 @@
       <c r="D31" t="s">
         <v>7</v>
       </c>
-      <c r="E31" t="s">
-        <v>41</v>
+      <c r="E31" s="2" t="s">
+        <v>126</v>
       </c>
       <c r="F31" t="s">
-        <v>187</v>
+        <v>201</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B32" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C32" t="s">
         <v>6</v>
@@ -6626,19 +6636,19 @@
       <c r="D32" t="s">
         <v>7</v>
       </c>
-      <c r="E32" s="2" t="s">
-        <v>132</v>
+      <c r="E32" t="s">
+        <v>41</v>
       </c>
       <c r="F32" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
       <c r="B33" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C33" t="s">
         <v>6</v>
@@ -6647,15 +6657,15 @@
         <v>7</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>126</v>
+        <v>132</v>
       </c>
       <c r="F33" t="s">
-        <v>202</v>
+        <v>188</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>115</v>
+        <v>122</v>
       </c>
       <c r="B34" t="b">
         <v>1</v>
@@ -6666,16 +6676,16 @@
       <c r="D34" t="s">
         <v>7</v>
       </c>
-      <c r="E34" t="s">
-        <v>90</v>
+      <c r="E34" s="2" t="s">
+        <v>126</v>
       </c>
       <c r="F34" t="s">
-        <v>189</v>
+        <v>202</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B35" t="b">
         <v>1</v>
@@ -6687,18 +6697,18 @@
         <v>7</v>
       </c>
       <c r="E35" t="s">
-        <v>41</v>
+        <v>90</v>
       </c>
       <c r="F35" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B36" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C36" t="s">
         <v>6</v>
@@ -6706,19 +6716,19 @@
       <c r="D36" t="s">
         <v>7</v>
       </c>
-      <c r="E36" s="2" t="s">
-        <v>132</v>
+      <c r="E36" t="s">
+        <v>41</v>
       </c>
       <c r="F36" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="B37" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C37" t="s">
         <v>6</v>
@@ -6727,17 +6737,37 @@
         <v>7</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>126</v>
+        <v>132</v>
       </c>
       <c r="F37" t="s">
-        <v>203</v>
+        <v>191</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
+        <v>123</v>
+      </c>
+      <c r="B38" t="b">
+        <v>1</v>
+      </c>
+      <c r="C38" t="s">
+        <v>6</v>
+      </c>
+      <c r="D38" t="s">
+        <v>7</v>
+      </c>
+      <c r="E38" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="F38" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
         <v>118</v>
       </c>
-      <c r="F38" t="s">
+      <c r="F39" t="s">
         <v>192</v>
       </c>
     </row>

</xml_diff>